<commit_message>
Updated test cases for testcase between 5 to 9
</commit_message>
<xml_diff>
--- a/data/TC03_checkindate.xlsx
+++ b/data/TC03_checkindate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>UserName</t>
   </si>
@@ -64,10 +64,16 @@
     <t>1 - One</t>
   </si>
   <si>
-    <t>25/05/2016</t>
-  </si>
-  <si>
-    <t>23/05/2016</t>
+    <t>28/05/2016</t>
+  </si>
+  <si>
+    <t>26/05/2016</t>
+  </si>
+  <si>
+    <t>Check in Error</t>
+  </si>
+  <si>
+    <t>Check-In Date shall be before than Check-Out Date</t>
   </si>
 </sst>
 </file>
@@ -103,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,24 +416,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,8 +468,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -477,10 +491,10 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I2" t="s">
@@ -488,6 +502,9 @@
       </c>
       <c r="J2" t="s">
         <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>